<commit_message>
changed terminal direction shrunk board size
</commit_message>
<xml_diff>
--- a/Hardware/PCB Design/Fabrication/2014_08_14/BOM.xlsx
+++ b/Hardware/PCB Design/Fabrication/2014_08_14/BOM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\B-Drive\School\Research\CBLA-Test-Bed-Hardware\PCB Design\Fabrication\2014_08_14\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\B-Drive\School\Research\CBLA-Test-Bed\Hardware\PCB Design\Fabrication\2014_08_14\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tentacle Module" sheetId="1" r:id="rId1"/>
@@ -723,7 +723,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1039,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,7 +1058,7 @@
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1279,7 +1279,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1325,7 +1325,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1529,6 +1529,7 @@
         <v>95</v>
       </c>
     </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1723,7 +1724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -2122,8 +2123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated the BOM with new components
</commit_message>
<xml_diff>
--- a/Hardware/PCB Design/Fabrication/2014_08_14/BOM.xlsx
+++ b/Hardware/PCB Design/Fabrication/2014_08_14/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Tentacle Module" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="167">
   <si>
     <t>Qty</t>
   </si>
@@ -617,6 +617,9 @@
   </si>
   <si>
     <t>S7005-ND, S7036-ND, S6100-ND</t>
+  </si>
+  <si>
+    <t>609-1046-ND, AE10396-ND</t>
   </si>
 </sst>
 </file>
@@ -723,7 +726,7 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1039,10 +1042,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,7 +1061,7 @@
     <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>3</v>
       </c>
@@ -1104,7 +1107,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>6</v>
       </c>
@@ -1124,7 +1127,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
@@ -1147,7 +1150,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1170,7 +1173,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1193,7 +1196,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1213,7 +1216,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1256,7 +1259,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1279,7 +1282,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1302,7 +1305,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1325,7 +1328,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1348,7 +1351,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1371,7 +1374,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -1394,7 +1397,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -1417,7 +1420,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>4</v>
       </c>
@@ -1440,7 +1443,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1480,10 +1483,10 @@
         <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1506,7 +1509,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1529,7 +1532,6 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1724,7 +1726,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>